<commit_message>
Corrección menor en solicitud
Se cambian unas palabras en unas ilustraciones
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado09/guion03/SolicitudGrafica_CN_09_03_CO_REC80.xlsx
+++ b/fuentes/contenidos/grado09/guion03/SolicitudGrafica_CN_09_03_CO_REC80.xlsx
@@ -605,27 +605,9 @@
     <t>Hombre negro y su hijo</t>
   </si>
   <si>
-    <t>Texto premisas</t>
-  </si>
-  <si>
-    <t>Texto Mecanismos</t>
-  </si>
-  <si>
-    <t>Texto Conclusiones</t>
-  </si>
-  <si>
     <t>Ver comentarios</t>
   </si>
   <si>
-    <t>Hacer un texto que diga premisas</t>
-  </si>
-  <si>
-    <t>Hacer un texto que diga mecanismos</t>
-  </si>
-  <si>
-    <t>Hacer un texro que diga concluiones</t>
-  </si>
-  <si>
     <t>Cachorros de perro</t>
   </si>
   <si>
@@ -635,9 +617,6 @@
     <t>Leones cazando</t>
   </si>
   <si>
-    <t>Hacer un grupo de arbustos, todos similares entre sí, excepto uno que tiene espinas. Hay venados comiendo de los arbustos, y cerca al espinoso, un venado que no endcuentra como comer. Luego, hacer una flecha a la derecha y  otro dibujo similar, pero ya no con un arbusto espinoso, sino tres.</t>
-  </si>
-  <si>
     <t>Ilustración</t>
   </si>
   <si>
@@ -663,6 +642,27 @@
   </si>
   <si>
     <t>Usar las dos imágenes, sin modificar, una al lado de la otra.</t>
+  </si>
+  <si>
+    <t>Premisas y conclusión</t>
+  </si>
+  <si>
+    <t>Hacer un texto que diga Premisas y conclusión</t>
+  </si>
+  <si>
+    <t>Hacer un texto que diga Mecanismo evolutivo</t>
+  </si>
+  <si>
+    <t>Mecanismo evolutivo</t>
+  </si>
+  <si>
+    <t>Implicaciones</t>
+  </si>
+  <si>
+    <t>Hacer un texro que diga Implicaciones</t>
+  </si>
+  <si>
+    <t>Hacer un grupo de arbustos, todos similares entre sí, excepto uno que tiene espinas. Hay venados comiendo de los arbustos, y cerca al espinoso, un venado que no encuentra como comer. Luego, hacer una flecha a la derecha y  otro dibujo similar, pero ya no con un arbusto espinoso, sino tres.</t>
   </si>
 </sst>
 </file>
@@ -2539,8 +2539,8 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2828,20 +2828,20 @@
         <v>M10B</v>
       </c>
     </row>
-    <row r="10" spans="1:16" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="str">
         <f>IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),"IMG01","")</f>
         <v>IMG01</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Recurso F7B</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E10" s="63" t="s">
         <v>165</v>
@@ -2863,10 +2863,10 @@
         <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="K10" s="64" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="O10" s="2" t="str">
         <f>'Definición técnica de imagenes'!A12</f>
@@ -2879,14 +2879,14 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F7B</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>165</v>
@@ -2908,10 +2908,10 @@
         <v/>
       </c>
       <c r="J11" s="64" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="K11" s="65" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
@@ -2924,14 +2924,14 @@
         <v>IMG03</v>
       </c>
       <c r="B12" s="62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F7B</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>165</v>
@@ -2953,10 +2953,10 @@
         <v/>
       </c>
       <c r="J12" s="64" t="s">
-        <v>194</v>
+        <v>209</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>198</v>
+        <v>210</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
@@ -3041,7 +3041,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J14" s="64" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K14" s="64"/>
       <c r="O14" s="2" t="str">
@@ -3084,7 +3084,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J15" s="66" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="K15" s="66"/>
       <c r="O15" s="2" t="str">
@@ -3127,7 +3127,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K16" s="64"/>
       <c r="O16" s="2" t="str">
@@ -3141,14 +3141,14 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F7B</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E17" s="63" t="s">
         <v>155</v>
@@ -3170,10 +3170,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="K17" s="66" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3186,14 +3186,14 @@
         <v>IMG09</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F7B</v>
       </c>
       <c r="D18" s="63" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E18" s="63" t="s">
         <v>155</v>
@@ -3215,10 +3215,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J18" s="66" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="K18" s="64" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3231,7 +3231,7 @@
         <v>IMG10</v>
       </c>
       <c r="B19" s="62" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="C19" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3260,10 +3260,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J19" s="67" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="K19" s="68" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
@@ -3276,14 +3276,14 @@
         <v>IMG11</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F7B</v>
       </c>
       <c r="D20" s="63" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="E20" s="63" t="s">
         <v>155</v>
@@ -3305,10 +3305,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J20" s="64" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="K20" s="66" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>

</xml_diff>